<commit_message>
update html, js, css, and xlsx files
</commit_message>
<xml_diff>
--- a/data/practice-tracker.xlsx
+++ b/data/practice-tracker.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalco\Documents\Projects\Fitness-tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{332EBC41-9B74-42D9-B9AE-490557587FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D03B450-C4F6-4167-AE3C-D2431CC69401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="1335" windowWidth="23310" windowHeight="14865" xr2:uid="{2049BC8B-3C7C-4D00-A2ED-7C4FD36DDDB1}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="23310" windowHeight="14865" xr2:uid="{2049BC8B-3C7C-4D00-A2ED-7C4FD36DDDB1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="active" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -86,11 +86,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -409,7 +406,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,45 +416,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
         <v>45334</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
         <v>45335</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="1">
         <v>45336</v>
       </c>
       <c r="C4" t="s">

</xml_diff>

<commit_message>
update app.py to read excel and put data into data.json
</commit_message>
<xml_diff>
--- a/data/practice-tracker.xlsx
+++ b/data/practice-tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalco\Documents\Projects\Fitness-tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D03B450-C4F6-4167-AE3C-D2431CC69401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1554435F-CBE1-4CD9-9339-2B5FA4EE6AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="735" windowWidth="23310" windowHeight="14865" xr2:uid="{2049BC8B-3C7C-4D00-A2ED-7C4FD36DDDB1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -51,12 +51,18 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,7 +94,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,20 +409,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15736F35-CA00-4BE1-B583-D654EE5FCF35}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -433,11 +439,14 @@
       <c r="A2" s="1">
         <v>45334</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -447,6 +456,9 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
@@ -455,8 +467,28 @@
       <c r="A4" s="1">
         <v>45336</v>
       </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
       <c r="C4" t="s">
         <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45337</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data in db
</commit_message>
<xml_diff>
--- a/data/practice-tracker.xlsx
+++ b/data/practice-tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalco\Documents\Projects\Fitness-tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1554435F-CBE1-4CD9-9339-2B5FA4EE6AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167FF884-1719-4612-BEB4-3529D1A904C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="735" windowWidth="23310" windowHeight="14865" xr2:uid="{2049BC8B-3C7C-4D00-A2ED-7C4FD36DDDB1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
@@ -49,19 +49,13 @@
   <si>
     <t>Double-unders</t>
   </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -94,7 +88,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +406,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,42 +447,42 @@
       <c r="A3" s="1">
         <v>45335</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45336</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45337</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update CrossFit content and data
</commit_message>
<xml_diff>
--- a/data/practice-tracker.xlsx
+++ b/data/practice-tracker.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalco\Documents\Projects\Fitness-tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167FF884-1719-4612-BEB4-3529D1A904C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E9F8D3-DA10-4CC2-A622-659DC7CA0086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="23310" windowHeight="14865" xr2:uid="{2049BC8B-3C7C-4D00-A2ED-7C4FD36DDDB1}"/>
+    <workbookView xWindow="2175" yWindow="930" windowWidth="23310" windowHeight="14865" activeTab="1" xr2:uid="{2049BC8B-3C7C-4D00-A2ED-7C4FD36DDDB1}"/>
   </bookViews>
   <sheets>
-    <sheet name="active" sheetId="1" r:id="rId1"/>
+    <sheet name="practiceTracker" sheetId="1" r:id="rId1"/>
+    <sheet name="crossfitStats" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -48,6 +49,24 @@
   </si>
   <si>
     <t>Double-unders</t>
+  </si>
+  <si>
+    <t>Skill</t>
+  </si>
+  <si>
+    <t>Stat</t>
+  </si>
+  <si>
+    <t>Deadlift</t>
+  </si>
+  <si>
+    <t>225lbs</t>
+  </si>
+  <si>
+    <t>Bench 1x3</t>
+  </si>
+  <si>
+    <t>125lbs</t>
   </si>
 </sst>
 </file>
@@ -86,9 +105,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,7 +425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15736F35-CA00-4BE1-B583-D654EE5FCF35}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -488,4 +508,52 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0653EBDA-935F-4477-AA9E-3EA3A31760AC}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2">
+        <v>44927</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>